<commit_message>
update literature (automatic + manual)
</commit_message>
<xml_diff>
--- a/scripts/script_data/manual_check_20240205.xlsx
+++ b/scripts/script_data/manual_check_20240205.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Z213165\Documents\PhD\github\Literature\scripts\script_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D3E5BC4-ED34-41F0-9D67-3F90D6139D0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCD4489B-A1D0-4E8E-BAB3-44785E5EE330}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13872" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="61">
   <si>
     <t>bibkey</t>
   </si>
@@ -199,7 +199,10 @@
     <t>38281317</t>
   </si>
   <si>
-    <t>add manually</t>
+    <t>[add manually]</t>
+  </si>
+  <si>
+    <t>[add new item]</t>
   </si>
 </sst>
 </file>
@@ -575,8 +578,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -653,7 +656,7 @@
       <c r="B2" t="s">
         <v>21</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D2">
@@ -716,7 +719,7 @@
         <v>37</v>
       </c>
       <c r="D3">
-        <v>0.60504201680672265</v>
+        <v>0.60504201680672298</v>
       </c>
       <c r="G3" t="s">
         <v>38</v>
@@ -808,12 +811,13 @@
         <v>34</v>
       </c>
       <c r="T4" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C3" r:id="rId1" xr:uid="{BD3AC8FE-C8E9-41DF-B6AD-42F6277FEC3A}"/>
+    <hyperlink ref="C2" r:id="rId2" xr:uid="{14148168-16E8-498C-9A45-557EAD6B519E}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>